<commit_message>
Clean up and create final report versions
</commit_message>
<xml_diff>
--- a/example-project/CY2D6-RQ/Parameters/Plots.xlsx
+++ b/example-project/CY2D6-RQ/Parameters/Plots.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esqlabs.sharepoint.com/sites/S-Parexel-P23-128-2D6Qualification/Freigegebene Dokumente/General/V00.01/Parameters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR.reports\example-project\CY2D6-RQ\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{2F14ED57-52C2-4837-9883-90432DF27DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{035E1E34-CA54-4110-8EB8-169A5A0943F1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06AD5DE-A535-4EAE-9B25-31C61F82CCE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataCombined" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DataCombined!$A$1:$C$83</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1861" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1259" uniqueCount="464">
   <si>
     <t>DataCombinedName</t>
   </si>
@@ -1178,720 +1178,108 @@
     <t>Sindrup (1992) - paroxetine hydrochloride, 30 mg, po, md, n=8 (PM) - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Sindrup (1992) - paroxetine hydrochloride, 30 mg, po, md, n=8 (PM)-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Sindrup (1992) - paroxetine hydrochloride, 30 mg, po, md, n=8 (PM)</t>
-  </si>
-  <si>
-    <t>Organism|PeripheralVenousBlood|Paroxetine|Plasma (Peripheral Venous Blood)</t>
-  </si>
-  <si>
-    <t>SI92_PO_30_PAR_MD_PM_56-PAROXETINE-Peripheral Venous Blood-Plasma-ng/mL</t>
-  </si>
-  <si>
-    <t>Sindrup (1992) - paroxetine hydrochloride, 30 mg, po, md, n=8 (PM), paroxetine (last dose)</t>
-  </si>
-  <si>
-    <t>SI92_PO_30_PAR_SD_PM_56-PAROXETINE-Peripheral Venous Blood-Plasma-ng/mL</t>
-  </si>
-  <si>
-    <t>Sindrup (1992) - paroxetine hydrochloride, 30 mg, po, md, n=8 (PM), paroxetine (first dose)</t>
-  </si>
-  <si>
     <t>Sindrup (1992) - paroxetine hydrochloride, 30 mg, po, md, n=9 (EM) - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Sindrup (1992) - paroxetine hydrochloride, 30 mg, po, md, n=9 (EM)-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Sindrup (1992) - paroxetine hydrochloride, 30 mg, po, md, n=9 (EM)</t>
-  </si>
-  <si>
-    <t>S92_PO_MD_EM-PAROXETINE-Peripheral Venous Blood-Plasma-ng/mL</t>
-  </si>
-  <si>
-    <t>Sindrup (1992) - paroxetine hydrochloride, 30 mg, po, md, n=9 (EM), paroxetine (last dose)</t>
-  </si>
-  <si>
-    <t>S92_PO_SD_EM-PAROXETINE-Peripheral Venous Blood-Plasma-ng/mL</t>
-  </si>
-  <si>
-    <t>Sindrup (1992) - paroxetine hydrochloride, 30 mg, po, md, n=9 (EM), paroxetine (first dose)</t>
-  </si>
-  <si>
-    <t>Sindrup (1992) - paroxetine hydrochloride, 30 mg, po, md, n=9 (EM)-Paroxetine-Kidney-Urine-Fraction excreted to urine</t>
-  </si>
-  <si>
-    <t>Organism|Kidney|Urine|Paroxetine|Fraction excreted to urine</t>
-  </si>
-  <si>
     <t>Massaroti (2005) - paroxetine hydrochloride, 20 mg, po, n=28 (EM) - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Massaroti (2005) - paroxetine hydrochloride, 20 mg, po, n=28 (EM)-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Massaroti (2005) - paroxetine hydrochloride, 20 mg, po, n=28 (EM)</t>
-  </si>
-  <si>
-    <t>MA05_PO_20_PAR_SD_PVB_NULL_61-PAROXETINE-Peripheral Venous Blood-Plasma-ng/mL</t>
-  </si>
-  <si>
-    <t>Massaroti (2005) - paroxetine hydrochloride, 20 mg, po, n=28 (EM), paroxetine</t>
-  </si>
-  <si>
     <t>Segura (2005) - paroxetine hydrochloride, 20 mg, po, md, n=7 (EM) - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Segura (2005) - paroxetine hydrochloride, 20 mg, po, md, n=7 (EM)-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Segura (2005) - paroxetine hydrochloride, 20 mg, po, md, n=7 (EM)</t>
-  </si>
-  <si>
-    <t>SE05_PO_20_PAR_MD_PVB_EM_67-Paroxetine-Peripheral Venous Blood-Plasma-ng/mL</t>
-  </si>
-  <si>
-    <t>Segura (2005) - paroxetine hydrochloride, 20 mg, po, md, n=7 (EM), paroxetine</t>
-  </si>
-  <si>
     <t>Calvo (2004) - paroxetine hydrochloride, 20 mg, po, md, n=25 (EM) - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Calvo (2004) - paroxetine hydrochloride, 20 mg, po, md, n=25 (EM)-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Calvo (2004) - paroxetine hydrochloride, 20 mg, po, md, n=25 (EM)</t>
-  </si>
-  <si>
-    <t>CA04_PO_20_PAR_MD_PVB_NULL_97-Paroxetine-Peripheral Venous Blood-Plasma-ng/mL</t>
-  </si>
-  <si>
-    <t>Calvo (2004) - paroxetine hydrochloride, 20 mg, po, md, n=25 (EM), paroxetine</t>
-  </si>
-  <si>
     <t>Belle (2002) - paroxetine hydrochloride, 20 mg, po, md, n=22 (EM) - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Belle (2002) - paroxetine hydrochloride, 20 mg, po, md, n=22 (EM)-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Belle (2002) - paroxetine hydrochloride, 20 mg, po, md, n=22 (EM)</t>
-  </si>
-  <si>
-    <t>BE02_PO_20_PAR_MD_PVB_EM_59-Paroxetine-Peripheral Venous Blood-Plasma-ng/mL</t>
-  </si>
-  <si>
-    <t>Belle (2002) - paroxetine hydrochloride, 20 mg, po, md, n=22 (EM), paroxetine</t>
-  </si>
-  <si>
     <t>McClelland (1985) - paroxetine hydrochloride, 70 mg, po, n=5 (EM) - Time Profile Analysis</t>
   </si>
   <si>
-    <t>McClelland (1985) - paroxetine hydrochloride, 70 mg, po, n=5 (EM)-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>McClelland (1985) - paroxetine hydrochloride, 70 mg, po, n=5 (EM)</t>
-  </si>
-  <si>
-    <t>MC85_PO_70_PAR_SD_PVB_NULL_99-Paroxetine-Peripheral Venous Blood-Plasma-ng/mL</t>
-  </si>
-  <si>
-    <t>McClelland (1985) paroxetine hydrochloride, 70 mg, po, n=5 (EM), paroxetine</t>
-  </si>
-  <si>
     <t>Schoedel (2012) - paroxetine hydrochloride, 20 mg, po, md, n=14 (EM) - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Schoedel (2012) - paroxetine hydrochloride, 20 mg, po, md, n=14 (EM)-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Schoedel (2012) - paroxetine hydrochloride, 20 mg, po, md, n=14 (EM)</t>
-  </si>
-  <si>
-    <t>SC12_PO_20_PAR_SD_PVB_EM_100-Paroxetine-Peripheral Venous Blood-Plasma-ng/mL</t>
-  </si>
-  <si>
-    <t>Schoedel (2012) - paroxetine hydrochloride, 20 mg, po, md, n=14 (EM), paroxetine</t>
-  </si>
-  <si>
     <t>Yasui-Furukori (2007) - paroxetine hydrochloride, 20 mg, po, n=12 (AS=1.25) - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Yasui-Furukori (2007) - paroxetine hydrochloride, 20 mg, po, n=12 (AS=1.25)-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Yasui-Furukori (2007) - paroxetine hydrochloride, 20 mg, po, n=12 (AS=1.25)</t>
-  </si>
-  <si>
-    <t>YA07_PO_20_PAR_SD_PVB_SEM_57-Paroxetine-Peripheral Venous Blood-Plasma-ng/mL</t>
-  </si>
-  <si>
-    <t>Yasui-Furukori (2007) - paroxetine hydrochloride, 20 mg, po, n=12 (AS=1.25), paroxetine</t>
-  </si>
-  <si>
     <t>Yasui-Furukori (2007) - paroxetine hydrochloride, 20 mg, po, n=13 (EM) - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Yasui-Furukori (2007) - paroxetine hydrochloride, 20 mg, po, n=13 (EM)-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Yasui-Furukori (2007) - paroxetine hydrochloride, 20 mg, po, n=13 (EM)</t>
-  </si>
-  <si>
-    <t>YS07_PO_20_PAR_SD_PVB_NULL_58-Paroxetine-Peripheral Venous Blood-Plasma-ng/mL</t>
-  </si>
-  <si>
-    <t>Yasui-Furukori (2007) - paroxetine hydrochloride, 20 mg, po, n=13 (EM), paroxetine</t>
-  </si>
-  <si>
     <t>Chen (2015) - paroxetine hydrochloride, 25 mg, po, n=4 (AS=0.5) - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Chen (2015) - paroxetine hydrochloride, 25 mg, po, n=4 (AS=0.5)-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Chen (2015) - paroxetine hydrochloride, 25 mg, po, n=4 (AS=0.5)</t>
-  </si>
-  <si>
-    <t>CH15_PO_20_PAR_SD_PVB_IM_134-Paroxetine-Peripheral Venous Blood-Plasma-[ng/mL]</t>
-  </si>
-  <si>
-    <t>Chen (2015) - paroxetine hydrochloride, 25 mg, po, n=4 (AS=0.5), paroxetine</t>
-  </si>
-  <si>
     <t>Chen (2015) - paroxetine hydrochloride, 25 mg, po, n=4 (AS=2) - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Chen (2015) - paroxetine hydrochloride, 25 mg, po, n=4 (AS=2)-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Chen (2015) - paroxetine hydrochloride, 25 mg, po, n=4 (AS=2)</t>
-  </si>
-  <si>
-    <t>CH15_PO_20_PAR_SD_PVB_EM_131-Paroxetine-Peripheral Venous Blood-Plasma-[ng/mL]</t>
-  </si>
-  <si>
-    <t>Chen (2015) - paroxetine hydrochloride, 25 mg, po, n=4 (AS=2), paroxetine</t>
-  </si>
-  <si>
     <t>Chen (2015) - paroxetine hydrochloride, 25 mg, po, n=5 (AS=1.5) - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Chen (2015) - paroxetine hydrochloride, 25 mg, po, n=5 (AS=1.5)-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Chen (2015) - paroxetine hydrochloride, 25 mg, po, n=5 (AS=1.5)</t>
-  </si>
-  <si>
-    <t>CH15_PO_20_PAR_SD_PVB_EM_132-Paroxetine-Peripheral Venous Blood-Plasma-[ng/mL]</t>
-  </si>
-  <si>
-    <t>Chen (2015) - paroxetine hydrochloride, 25 mg, po, n=5 (AS=1.5), paroxetine</t>
-  </si>
-  <si>
     <t>Chen (2015) - paroxetine hydrochloride, 25 mg, po, n=11 (AS=1) - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Chen (2015) - paroxetine hydrochloride, 25 mg, po, n=11 (AS=1)-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Chen (2015) - paroxetine hydrochloride, 25 mg, po, n=11 (AS=1)</t>
-  </si>
-  <si>
-    <t>CH15_PO_20_PAR_SD_PVB_EM_133-Paroxetine-Peripheral Venous Blood-Plasma-[ng/mL]</t>
-  </si>
-  <si>
-    <t>Chen (2015) - paroxetine hydrochloride, 25 mg, po, n=11 (AS=1), paroxetine</t>
-  </si>
-  <si>
     <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=3 (AS=3) - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=3 (AS=3)-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=3 (AS=3)</t>
-  </si>
-  <si>
-    <t>MUXX_PO_40_PAR_MD_PVB_UM_145-Paroxetine-Peripheral Venous Blood-Plasma-[ng/mL]</t>
-  </si>
-  <si>
-    <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=3 (AS=3), paroxetine</t>
-  </si>
-  <si>
     <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=3 (AS=2) - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=3 (AS=2)-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=3 (AS=2)</t>
-  </si>
-  <si>
-    <t>MUXX_PO_40_PAR_MD_PVB_EM_146-Paroxetine-Peripheral Venous Blood-Plasma-[ng/mL]</t>
-  </si>
-  <si>
-    <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=3 (AS=2), paroxetine</t>
-  </si>
-  <si>
     <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=3 (AS=0) - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=3 (AS=0)-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=3 (AS=0)</t>
-  </si>
-  <si>
-    <t>MUXX_PO_40_PAR_MD_PVB_PM_150-Paroxetine-Peripheral Venous Blood-Plasma-[ng/mL]</t>
-  </si>
-  <si>
-    <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=3 (AS=0), paroxetine</t>
-  </si>
-  <si>
     <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=2 (AS=1) - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=2 (AS=1)-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=2 (AS=1)</t>
-  </si>
-  <si>
-    <t>MUXX_PO_40_PAR_MD_PVB_IM_147-Paroxetine-Peripheral Venous Blood-Plasma-[ng/mL]</t>
-  </si>
-  <si>
-    <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=2 (AS=1), paroxetine</t>
-  </si>
-  <si>
     <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=4 (AS=0.5) - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=4 (AS=0.5)-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=4 (AS=0.5)</t>
-  </si>
-  <si>
-    <t>MUXX_PO_40_PAR_MD_PVB_IM_149-Paroxetine-Peripheral Venous Blood-Plasma-[ng/mL]</t>
-  </si>
-  <si>
-    <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=4 (AS=0.5), paroxetine</t>
-  </si>
-  <si>
     <t>Lund (1982) - paroxetine hydrochloride, 23 mg, iv, n=1 (EM), D - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 23 mg, iv, n=1 (EM), D</t>
-  </si>
-  <si>
-    <t>LU82_IV_23_PAR_SD_PVB_NULL_45-Paroxetine-Peripheral Venous Blood-Plasma-[ng/mL]</t>
-  </si>
-  <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 23 mg, iv, n=1 (EM), D, paroxetine</t>
-  </si>
-  <si>
     <t>Lund (1982) - paroxetine hydrochloride, 28 mg, iv, n=1 (EM), A - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 28 mg, iv, n=1 (EM), A-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 28 mg, iv, n=1 (EM), A</t>
-  </si>
-  <si>
-    <t>LU82_IV_28_PAR_SD_PVB_NULL_42-Paroxetine-Peripheral Venous Blood-Plasma-[ng/mL]</t>
-  </si>
-  <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 28 mg, iv, n=1 (EM), A, paroxetine</t>
-  </si>
-  <si>
     <t>Lund (1982) - paroxetine hydrochloride, 28 mg, iv, n=1 (EM), B - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 28 mg, iv, n=1 (EM), B-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 28 mg, iv, n=1 (EM), B</t>
-  </si>
-  <si>
-    <t>LU82_IV_28_PAR_SD_PVB_NULL_43-Paroxetine-Peripheral Venous Blood-Plasma-[ng/mL]</t>
-  </si>
-  <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 28 mg, iv, n=1 (EM), B, paroxetine</t>
-  </si>
-  <si>
     <t>Lund (1982) - paroxetine hydrochloride, 28 mg, iv, n=1 (EM), C - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 28 mg, iv, n=1 (EM), C-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 28 mg, iv, n=1 (EM), C</t>
-  </si>
-  <si>
-    <t>LU82_IV_28_PAR_SD_PVB_NULL_44-Paroxetine-Peripheral Venous Blood-Plasma-[ng/mL]</t>
-  </si>
-  <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 28 mg, iv, n=1 (EM), C, paroxetine</t>
-  </si>
-  <si>
     <t>Lund (1982) - paroxetine hydrochloride, 45 mg, po, n=1 (EM), A - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 45 mg, po, n=1 (EM), A-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 45 mg, po, n=1 (EM), A</t>
-  </si>
-  <si>
-    <t>LU82_PO_45_PAR_SD_PVB_NULL_42-Paroxetine-Peripheral Venous Blood-Plasma-[ng/mL]</t>
-  </si>
-  <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 45 mg, po, n=1 (EM), A, paroxetine</t>
-  </si>
-  <si>
     <t>Lund (1982) - paroxetine hydrochloride, 45 mg, po, n=1 (EM), B - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 45 mg, po, n=1 (EM), B-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 45 mg, po, n=1 (EM), B</t>
-  </si>
-  <si>
-    <t>LU82_PO_45_PAR_SD_PVB_NULL_43-Paroxetine-Peripheral Venous Blood-Plasma-[ng/mL]</t>
-  </si>
-  <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 45 mg, po, n=1 (EM), B, paroxetine</t>
-  </si>
-  <si>
     <t>Lund (1982) - paroxetine hydrochloride, 45 mg, po, n=1 (EM), C - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 45 mg, po, n=1 (EM), C-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 45 mg, po, n=1 (EM), C</t>
-  </si>
-  <si>
-    <t>LU82_PO_45_PAR_SD_PVB_NULL_44-Paroxetine-Peripheral Venous Blood-Plasma-[ng/mL]</t>
-  </si>
-  <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 45 mg, po, n=1 (EM), C, paroxetine</t>
-  </si>
-  <si>
     <t>Lund (1982) - paroxetine hydrochloride, 45 mg, po, n=1 (EM), D - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 45 mg, po, n=1 (EM), D</t>
-  </si>
-  <si>
-    <t>LU82_PO_45_PAR_SD_PVB_NULL_45-Paroxetine-Peripheral Venous Blood-Plasma-[ng/mL]</t>
-  </si>
-  <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 45 mg, po, n=1 (EM), D, paroxetine</t>
-  </si>
-  <si>
     <t>Yoon (2000) - paroxetine hydrochloride, 40 mg, po, n=6 (AS=2) - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Yoon (2000) - paroxetine hydrochloride, 40 mg, po, n=6 (AS=2)-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Yoon (2000) - paroxetine hydrochloride, 40 mg, po, n=6 (AS=2)</t>
-  </si>
-  <si>
-    <t>YO00_PO_40_PAR_SD_PVB_EM_151-Paroxetine-Peripheral Venous Blood-Plasma-[ng/mL]</t>
-  </si>
-  <si>
-    <t>Yoon (2000) - paroxetine hydrochloride, 40 mg, po, n=6 (AS=2), paroxetine</t>
-  </si>
-  <si>
     <t>Yoon (2000) - paroxetine hydrochloride, 40 mg, po, n=1 (AS=0) - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Yoon (2000) - paroxetine hydrochloride, 40 mg, po, n=1 (AS=0)-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Yoon (2000) - paroxetine hydrochloride, 40 mg, po, n=1 (AS=0)</t>
-  </si>
-  <si>
-    <t>YO00_PO_40_PAR_SD_PVB_PM_154-Paroxetine-Peripheral Venous Blood-Plasma-[ng/mL]</t>
-  </si>
-  <si>
-    <t>Yoon (2000) - paroxetine hydrochloride, 40 mg, po, n=1 (AS=0), paroxetine</t>
-  </si>
-  <si>
     <t>Yoon (2000) - paroxetine hydrochloride, 40 mg, po, n=3 (AS=0.5) - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Yoon (2000) - paroxetine hydrochloride, 40 mg, po, n=3 (AS=0.5)-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Yoon (2000) - paroxetine hydrochloride, 40 mg, po, n=3 (AS=0.5)</t>
-  </si>
-  <si>
-    <t>YO00_PO_40_PAR_SD_PVB_IM_153-Paroxetine-Peripheral Venous Blood-Plasma-[ng/mL]</t>
-  </si>
-  <si>
-    <t>Yoon (2000) - paroxetine hydrochloride, 40 mg, po, n=3 (AS=0.5), paroxetine</t>
-  </si>
-  <si>
     <t>Yoon (2000) - paroxetine hydrochloride, 40 mg, po, n=6 (AS=1.25) - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Yoon (2000) - paroxetine hydrochloride, 40 mg, po, n=6 (AS=1.25)-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Yoon (2000) - paroxetine hydrochloride, 40 mg, po, n=6 (AS=1.25)</t>
-  </si>
-  <si>
-    <t>YO00_PO_40_PAR_SD_PVB_EM_152-Paroxetine-Peripheral Venous Blood-Plasma-[ng/mL]</t>
-  </si>
-  <si>
-    <t>Yoon (2000) - paroxetine hydrochloride, 40 mg, po, n=6 (AS=1.25), paroxetine</t>
-  </si>
-  <si>
     <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=1 (AS=0.75) - Time Profile Analysis</t>
   </si>
   <si>
-    <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=1 (AS=0.75)-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=1 (AS=0.75)</t>
-  </si>
-  <si>
-    <t>MUXX_PO_40_PAR_MD_PVB_IM_148-Paroxetine-Peripheral Venous Blood-Plasma-[ng/mL]</t>
-  </si>
-  <si>
-    <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=1 (AS=0.75), paroxetine</t>
-  </si>
-  <si>
     <t>van der Lee (2007) - paroxetine hydrochloride, 20 mg, po, md, n=26 (EM) - Time Profile Analysis</t>
   </si>
   <si>
-    <t>van der Lee (2007) - paroxetine hydrochloride, 20 mg, po, md, n=26 (EM)-Paroxetine-Peripheral Venous Blood-Plasma-Concentration</t>
-  </si>
-  <si>
-    <t>van der Lee (2007) - paroxetine hydrochloride, 20 mg, po, md, n=26 (EM)</t>
-  </si>
-  <si>
-    <t>VA07_PO_20_PAR_MD_PVB_EM_60-Paroxetine-Peripheral Venous Blood-Plasma-ng/mL</t>
-  </si>
-  <si>
-    <t>van der Lee (2007) - paroxetine hydrochloride, 20 mg, po, md, n=26 (EM), paroxetine</t>
-  </si>
-  <si>
     <t>nmol/l</t>
   </si>
   <si>
-    <t>"Sindrup (1992) - paroxetine hydrochloride, 30 mg, po, md, n=8 (PM) - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Sindrup (1992) - paroxetine hydrochloride, 30 mg, po, md, n=8 (PM) - time profile</t>
-  </si>
-  <si>
-    <t>Sindrup (1992) - paroxetine hydrochloride, 30 mg, po, md, n=9 (EM) - time profile</t>
-  </si>
-  <si>
-    <t>"Massaroti (2005) - paroxetine hydrochloride, 20 mg, po, n=28 (EM) - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Massaroti (2005) - paroxetine hydrochloride, 20 mg, po, n=28 (EM) - time profile</t>
-  </si>
-  <si>
-    <t>"Segura (2005) - paroxetine hydrochloride, 20 mg, po, md, n=7 (EM) - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Segura (2005) - paroxetine hydrochloride, 20 mg, po, md, n=7 (EM) - time profile</t>
-  </si>
-  <si>
-    <t>"Calvo (2004) - paroxetine hydrochloride, 20 mg, po, md, n=25 (EM) - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Calvo (2004) - paroxetine hydrochloride, 20 mg, po, md, n=25 (EM) - time profile</t>
-  </si>
-  <si>
-    <t>"Belle (2002) - paroxetine hydrochloride, 20 mg, po, md, n=22 (EM) - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Belle (2002) - paroxetine hydrochloride, 20 mg, po, md, n=22 (EM) - time profile</t>
-  </si>
-  <si>
-    <t>"McClelland (1985) - paroxetine hydrochloride, 70 mg, po, n=5 (EM) - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>McClelland (1985) - paroxetine hydrochloride, 70 mg, po, n=5 (EM) - time profile</t>
-  </si>
-  <si>
-    <t>"Schoedel (2012) - paroxetine hydrochloride, 20 mg, po, md, n=14 (EM) - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Schoedel (2012) - paroxetine hydrochloride, 20 mg, po, md, n=14 (EM) - time profile</t>
-  </si>
-  <si>
-    <t>"Yasui-Furukori (2007) - paroxetine hydrochloride, 20 mg, po, n=12 (AS=1.25) - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Yasui-Furukori (2007) - paroxetine hydrochloride, 20 mg, po, n=12 (AS=1.25) - time profile</t>
-  </si>
-  <si>
-    <t>"Yasui-Furukori (2007) - paroxetine hydrochloride, 20 mg, po, n=13 (EM) - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Yasui-Furukori (2007) - paroxetine hydrochloride, 20 mg, po, n=13 (EM) - time profile</t>
-  </si>
-  <si>
-    <t>"Chen (2015) - paroxetine hydrochloride, 25 mg, po, n=4 (AS=0.5) - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Chen (2015) - paroxetine hydrochloride, 25 mg, po, n=4 (AS=0.5) - time profile</t>
-  </si>
-  <si>
-    <t>"Chen (2015) - paroxetine hydrochloride, 25 mg, po, n=4 (AS=2) - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Chen (2015) - paroxetine hydrochloride, 25 mg, po, n=4 (AS=2) - time profile</t>
-  </si>
-  <si>
-    <t>"Chen (2015) - paroxetine hydrochloride, 25 mg, po, n=5 (AS=1.5) - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Chen (2015) - paroxetine hydrochloride, 25 mg, po, n=5 (AS=1.5) - time profile</t>
-  </si>
-  <si>
-    <t>"Chen (2015) - paroxetine hydrochloride, 25 mg, po, n=11 (AS=1) - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Chen (2015) - paroxetine hydrochloride, 25 mg, po, n=11 (AS=1) - time profile</t>
-  </si>
-  <si>
-    <t>"Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=3 (AS=3) - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=3 (AS=3) - time profile</t>
-  </si>
-  <si>
-    <t>"Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=3 (AS=2) - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=3 (AS=2) - time profile</t>
-  </si>
-  <si>
-    <t>"Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=3 (AS=0) - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=3 (AS=0) - time profile</t>
-  </si>
-  <si>
-    <t>"Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=2 (AS=1) - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=2 (AS=1) - time profile</t>
-  </si>
-  <si>
-    <t>"Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=4 (AS=0.5) - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=4 (AS=0.5) - time profile</t>
-  </si>
-  <si>
-    <t>"Lund (1982) - paroxetine hydrochloride, 23 mg, iv, n=1 (EM), D - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 23 mg, iv, n=1 (EM), D - time profile</t>
-  </si>
-  <si>
-    <t>"Lund (1982) - paroxetine hydrochloride, 28 mg, iv, n=1 (EM), A - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 28 mg, iv, n=1 (EM), A - time profile</t>
-  </si>
-  <si>
-    <t>"Lund (1982) - paroxetine hydrochloride, 28 mg, iv, n=1 (EM), B - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 28 mg, iv, n=1 (EM), B - time profile</t>
-  </si>
-  <si>
-    <t>"Lund (1982) - paroxetine hydrochloride, 28 mg, iv, n=1 (EM), C - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 28 mg, iv, n=1 (EM), C - time profile</t>
-  </si>
-  <si>
-    <t>"Lund (1982) - paroxetine hydrochloride, 45 mg, po, n=1 (EM), A - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 45 mg, po, n=1 (EM), A - time profile</t>
-  </si>
-  <si>
-    <t>"Lund (1982) - paroxetine hydrochloride, 45 mg, po, n=1 (EM), B - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 45 mg, po, n=1 (EM), B - time profile</t>
-  </si>
-  <si>
-    <t>"Lund (1982) - paroxetine hydrochloride, 45 mg, po, n=1 (EM), C - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 45 mg, po, n=1 (EM), C - time profile</t>
-  </si>
-  <si>
-    <t>"Lund (1982) - paroxetine hydrochloride, 45 mg, po, n=1 (EM), D - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Lund (1982) - paroxetine hydrochloride, 45 mg, po, n=1 (EM), D - time profile</t>
-  </si>
-  <si>
-    <t>"Yoon (2000) - paroxetine hydrochloride, 40 mg, po, n=6 (AS=2) - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Yoon (2000) - paroxetine hydrochloride, 40 mg, po, n=6 (AS=2) - time profile</t>
-  </si>
-  <si>
-    <t>"Yoon (2000) - paroxetine hydrochloride, 40 mg, po, n=1 (AS=0) - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Yoon (2000) - paroxetine hydrochloride, 40 mg, po, n=1 (AS=0) - time profile</t>
-  </si>
-  <si>
-    <t>"Yoon (2000) - paroxetine hydrochloride, 40 mg, po, n=3 (AS=0.5) - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Yoon (2000) - paroxetine hydrochloride, 40 mg, po, n=3 (AS=0.5) - time profile</t>
-  </si>
-  <si>
-    <t>"Yoon (2000) - paroxetine hydrochloride, 40 mg, po, n=6 (AS=1.25) - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Yoon (2000) - paroxetine hydrochloride, 40 mg, po, n=6 (AS=1.25) - time profile</t>
-  </si>
-  <si>
-    <t>"Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=1 (AS=0.75) - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>Mürdter (2016) - paroxetine hydrochloride, 40 mg, po, md, n=1 (AS=0.75) - time profile</t>
-  </si>
-  <si>
-    <t>"van der Lee (2007) - paroxetine hydrochloride, 20 mg, po, md, n=26 (EM) - Time Profile Analysis"</t>
-  </si>
-  <si>
-    <t>van der Lee (2007) - paroxetine hydrochloride, 20 mg, po, md, n=26 (EM) - time profile</t>
-  </si>
-  <si>
     <t>Sindrup (1992) - paroxetine hydrochloride, 30 mg, po, md, n=9 (EM) - Fraction Excreted</t>
   </si>
   <si>
-    <t>"Sindrup (1992) - paroxetine hydrochloride, 30 mg, po, md, n=9 (EM) - Time Profile Analysis", "Sindrup (1992) - paroxetine hydrochloride, 30 mg, po, md, n=9 (EM) - Fraction Excreted"</t>
-  </si>
-  <si>
     <t>PVB</t>
   </si>
   <si>
@@ -1904,25 +1292,145 @@
     <t>NA07_PO_30_DEX_SD_PVB_EM_123-Dextromethorphan-Peripheral Venous Blood-Plasma-[ng/mL]_v11.2</t>
   </si>
   <si>
-    <t>Dextromethorpharm</t>
-  </si>
-  <si>
-    <t>Dextrorphan total</t>
-  </si>
-  <si>
     <t>160, 220</t>
   </si>
   <si>
-    <t>xAxisValuesLimits</t>
-  </si>
-  <si>
-    <t>yAxisValuesLimits</t>
-  </si>
-  <si>
-    <t>Dextromethorphan</t>
-  </si>
-  <si>
-    <t>Dextrorphan</t>
+    <t>CA96_PO_30_DEX_SD_PVB_EM_92-Dextromethorphan-Peripheral Venous Blood-Plasma-ng/mL v9.1</t>
+  </si>
+  <si>
+    <t>CA96_PO_30_DEX_SD_PVB_PM_93-Dextromethorphan-Peripheral Venous Blood-Plasma-ng/mL v9.1</t>
+  </si>
+  <si>
+    <t>DU05_IV_0.5_DEX_SD_PVB_NULL_89-Dextromethorphan-Peripheral Venous Blood-Plasma-ng/mL v9.1</t>
+  </si>
+  <si>
+    <t>GO04_PO_30_DEX_SD_PVB_PM_96-Dextromethorphan-Peripheral Venous Blood-Plasma-ng/mL v9.1</t>
+  </si>
+  <si>
+    <t>QI16_PO_15_DEX_SD_PVB_EM_124-Dextromethorphan-Peripheral Venous Blood-Plasma-[ng/mL] v9.1</t>
+  </si>
+  <si>
+    <t>QI16_PO_15_DEX_SD_PVB_EM_126-Dextromethorphan-Peripheral Venous Blood-Plasma-[ng/mL] v9.1</t>
+  </si>
+  <si>
+    <t>QI16_PO_15_DEX_SD_PVB_EM_125-Dextromethorphan-Peripheral Venous Blood-Plasma-[ng/mL] v9.1</t>
+  </si>
+  <si>
+    <t>ST18_PO_5_DEX_SD_PVB_NM_120-Dextromethorphan-Peripheral Venous Blood-Plasma-[ng/mL] v9.1</t>
+  </si>
+  <si>
+    <t>ST18_PO_5_DXT_SD_PVB_EM_120-Dextrorphan-Peripheral Venous Blood-Plasma-[ng/mL] v9.1</t>
+  </si>
+  <si>
+    <t>ED17_PO_30_DEX_SD_PVB_NULL_118-Dextromethorphan-Peripheral Venous Blood-Plasma-[ng/mL] v9.1</t>
+  </si>
+  <si>
+    <t>Dextromethorpharm v9.1</t>
+  </si>
+  <si>
+    <t>Dextrorphan total v9.1</t>
+  </si>
+  <si>
+    <t>NA07_PO_30_DEX_SD_PVB_EM_123-Dextromethorphan-Peripheral Venous Blood-Plasma-[ng/mL] v9.1</t>
+  </si>
+  <si>
+    <t>NA07_PO_30_DXT_SD_PVB_EM_123-Dextrorphan-Peripheral Venous Blood-Plasma-[ng/mL] v9.1</t>
+  </si>
+  <si>
+    <t>TE99_PO_80_DEX_SD_PVB_EM_122-Dextromethorphan-Peripheral Venous Blood-Plasma-[ng/mL] v9.1</t>
+  </si>
+  <si>
+    <t>TE99_PO_80_DXT_SD_PVB_EM_122-Dextrorphan-total-Peripheral Venous Blood-Plasma-[ng/mL] v9.1</t>
+  </si>
+  <si>
+    <t>YA17_PO_30_DEX_SD_PVB_EM_127-Dextromethorphan-Peripheral Venous Blood-Plasma-[ng/mL] v9.1</t>
+  </si>
+  <si>
+    <t>YA17_PO_30_DEX_SD_PVB_EM_128-Dextromethorphan-Peripheral Venous Blood-Plasma-[ng/mL] v9.1</t>
+  </si>
+  <si>
+    <t>NY08_PO_30_DEX_SD_PVB_EM_130-Dextromethorphan-Peripheral Venous Blood-Plasma-[ng/mL] v9.1</t>
+  </si>
+  <si>
+    <t>SC95_PO_30_DEX_SD_PVB_PM_91-Dextromethorphan-Peripheral Venous Blood-Plasma-ng/mL v9.1</t>
+  </si>
+  <si>
+    <t>ST18_PO_5_DEX_SD_PVB_IM_121-Dextromethorphan-Peripheral Venous Blood-Plasma-[ng/mL] v9.1</t>
+  </si>
+  <si>
+    <t>ST18_PO_5_DXT_SD_PVB_EM_121-Dextrorphan-Peripheral Venous Blood-Plasma-[ng/mL] v9.1</t>
+  </si>
+  <si>
+    <t>SC95_PO_30_DXT_SD_PVB_EM_90-Dextrorphan-Peripheral Venous Blood-Plasma-ng/mL v9.1</t>
+  </si>
+  <si>
+    <t>SC95_PO_30_DXG_SD_PVB_EM_90-Dextrorphan-O-glucuronide-Peripheral Venous Blood-Plasma-[ng/mL] v9.1</t>
+  </si>
+  <si>
+    <t>Patent_Dextromethorphan - Control-Dextromethorphan-Peripheral Venous Blood-Plasma-Conc   v9.1</t>
+  </si>
+  <si>
+    <t>Patent_Dextrorphan - Control-Dextrorphan-total-Peripheral Venous Blood-Plasma-Conc   v9.1</t>
+  </si>
+  <si>
+    <t>Dextromethorphan v9.1</t>
+  </si>
+  <si>
+    <t>Dextrorphan v9.1</t>
+  </si>
+  <si>
+    <t>SA14_PO_30_DEX_SD_PVB_NM_135-Dextromethorphan-Peripheral Venous Blood-Plasma-[ng/mL] v9.1</t>
+  </si>
+  <si>
+    <t>SA14_PO_30_DXT_SD_PVB_NM_135-Dextrorphan-Peripheral Venous Blood-Plasma-[ng/mL] v9.1</t>
+  </si>
+  <si>
+    <t>SA18_PO_30_DEX__PCO_NULL_137_DDI-Dextromethorphan-Peripheral Venous Blood-Plasma-[ng/mL] v9.1</t>
+  </si>
+  <si>
+    <t>AR17_PO_30_DEX_SD_PVB_NULL_136-Dextromethorphan-Peripheral Venous Blood-Plasma-[ng/mL] v9.1</t>
+  </si>
+  <si>
+    <t>DU10_PO_30_DEX__CVI_NULL_138_DDI-Dextromethorphan-Peripheral Venous Blood-Plasma-[ng/mL] v9.1</t>
+  </si>
+  <si>
+    <t>KA14_PO_30_DEX__CVI_EM_139_DDI-Dextromethorphan-Peripheral Venous Blood-Plasma-[ng/mL] v9.1</t>
+  </si>
+  <si>
+    <t>KA18_PO_30_DEX_SD_PVB_EM_129-Dextromethorphan-Peripheral Venous Blood-Plasma-[ng/mL] v9.1</t>
+  </si>
+  <si>
+    <t>GA18_PO_30_DEX_SD_PVB_NM_192-Dextromethorphan-Peripheral Venous Blood-Plasma-[ng/mL] v9.1</t>
+  </si>
+  <si>
+    <t>ER15_PO_30_DEX_SD_PVB_NULL_186-Dextromethorphan-Peripheral Venous Blood-Plasma-[ng/mL] v9.1</t>
+  </si>
+  <si>
+    <t>ER15_PO_30_DXT_SD_PVB_NULL_186-Dextrorphan-Peripheral Venous Blood-Plasma-[ng/mL] v9.1</t>
+  </si>
+  <si>
+    <t>Gorski 2004 EM, dextromethorphan, 30 mg dextromethorphan hydromide (capsule/solution), n=11-Dextromethorphan-Peripheral Venous Blood-Plasma-ng/mL v9.1</t>
+  </si>
+  <si>
+    <t>Gorski 2004 EM, dextrorphan, 30 mg dextromethorphan hydromide (capsule/solution), n=11-Dextrorphan-total-Peripheral Venous Blood-Plasma-[ng/mL] v9.1</t>
+  </si>
+  <si>
+    <t>Dextromethorpharm v11.2</t>
+  </si>
+  <si>
+    <t>Dextrorphan total v11.2</t>
+  </si>
+  <si>
+    <t>Dextromethorphan v11.2</t>
+  </si>
+  <si>
+    <t>Dextrorphan v11.2</t>
+  </si>
+  <si>
+    <t>xValuesLimits</t>
+  </si>
+  <si>
+    <t>yValuesLimits</t>
   </si>
 </sst>
 </file>
@@ -2279,12 +1787,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M195"/>
+  <dimension ref="A1:M125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="82" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="D1" zoomScale="82" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G59" sqref="G59"/>
+      <selection pane="bottomLeft" activeCell="G114" sqref="G114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2360,7 +1868,7 @@
         <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>418</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -2377,7 +1885,7 @@
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>418</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -2397,7 +1905,7 @@
         <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>419</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -2414,7 +1922,7 @@
         <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2434,7 +1942,7 @@
         <v>11</v>
       </c>
       <c r="G6" t="s">
-        <v>23</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -2451,7 +1959,7 @@
         <v>24</v>
       </c>
       <c r="G7" t="s">
-        <v>23</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -2471,7 +1979,7 @@
         <v>11</v>
       </c>
       <c r="G8" t="s">
-        <v>28</v>
+        <v>421</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -2488,7 +1996,7 @@
         <v>29</v>
       </c>
       <c r="G9" t="s">
-        <v>28</v>
+        <v>421</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -2508,7 +2016,7 @@
         <v>11</v>
       </c>
       <c r="G10" t="s">
-        <v>33</v>
+        <v>422</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -2525,7 +2033,7 @@
         <v>34</v>
       </c>
       <c r="G11" t="s">
-        <v>33</v>
+        <v>422</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -2545,7 +2053,7 @@
         <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>38</v>
+        <v>423</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -2562,7 +2070,7 @@
         <v>39</v>
       </c>
       <c r="G13" t="s">
-        <v>38</v>
+        <v>423</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -2582,7 +2090,7 @@
         <v>11</v>
       </c>
       <c r="G14" t="s">
-        <v>43</v>
+        <v>424</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -2599,7 +2107,7 @@
         <v>44</v>
       </c>
       <c r="G15" t="s">
-        <v>43</v>
+        <v>424</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -2619,7 +2127,7 @@
         <v>11</v>
       </c>
       <c r="G16" t="s">
-        <v>48</v>
+        <v>425</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2639,7 +2147,7 @@
         <v>50</v>
       </c>
       <c r="G17" t="s">
-        <v>51</v>
+        <v>426</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2656,7 +2164,7 @@
         <v>52</v>
       </c>
       <c r="G18" t="s">
-        <v>51</v>
+        <v>426</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2673,7 +2181,7 @@
         <v>53</v>
       </c>
       <c r="G19" t="s">
-        <v>48</v>
+        <v>425</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2693,7 +2201,7 @@
         <v>11</v>
       </c>
       <c r="G20" t="s">
-        <v>57</v>
+        <v>427</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -2710,7 +2218,7 @@
         <v>58</v>
       </c>
       <c r="G21" t="s">
-        <v>57</v>
+        <v>427</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -2730,7 +2238,7 @@
         <v>11</v>
       </c>
       <c r="G22" t="s">
-        <v>621</v>
+        <v>428</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -2750,7 +2258,7 @@
         <v>62</v>
       </c>
       <c r="G23" t="s">
-        <v>622</v>
+        <v>429</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2767,7 +2275,7 @@
         <v>64</v>
       </c>
       <c r="G24" t="s">
-        <v>622</v>
+        <v>429</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -2784,7 +2292,7 @@
         <v>66</v>
       </c>
       <c r="G25" t="s">
-        <v>621</v>
+        <v>428</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -2804,7 +2312,7 @@
         <v>11</v>
       </c>
       <c r="G26" t="s">
-        <v>71</v>
+        <v>430</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -2821,7 +2329,7 @@
         <v>72</v>
       </c>
       <c r="G27" t="s">
-        <v>71</v>
+        <v>430</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -2838,7 +2346,7 @@
         <v>73</v>
       </c>
       <c r="G28" t="s">
-        <v>70</v>
+        <v>431</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -2858,7 +2366,7 @@
         <v>50</v>
       </c>
       <c r="G29" t="s">
-        <v>70</v>
+        <v>431</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -2878,7 +2386,7 @@
         <v>11</v>
       </c>
       <c r="G30" t="s">
-        <v>78</v>
+        <v>432</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -2895,7 +2403,7 @@
         <v>79</v>
       </c>
       <c r="G31" t="s">
-        <v>78</v>
+        <v>432</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -2912,7 +2420,7 @@
         <v>81</v>
       </c>
       <c r="G32" t="s">
-        <v>80</v>
+        <v>433</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -2932,7 +2440,7 @@
         <v>62</v>
       </c>
       <c r="G33" t="s">
-        <v>80</v>
+        <v>433</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -2952,7 +2460,7 @@
         <v>11</v>
       </c>
       <c r="G34" t="s">
-        <v>85</v>
+        <v>434</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -2969,7 +2477,7 @@
         <v>86</v>
       </c>
       <c r="G35" t="s">
-        <v>85</v>
+        <v>434</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -2989,7 +2497,7 @@
         <v>11</v>
       </c>
       <c r="G36" t="s">
-        <v>90</v>
+        <v>435</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -3006,7 +2514,7 @@
         <v>91</v>
       </c>
       <c r="G37" t="s">
-        <v>90</v>
+        <v>435</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -3026,7 +2534,7 @@
         <v>11</v>
       </c>
       <c r="G38" t="s">
-        <v>94</v>
+        <v>436</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -3043,7 +2551,7 @@
         <v>95</v>
       </c>
       <c r="G39" t="s">
-        <v>94</v>
+        <v>436</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -3063,7 +2571,7 @@
         <v>11</v>
       </c>
       <c r="G40" t="s">
-        <v>99</v>
+        <v>437</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -3080,7 +2588,7 @@
         <v>100</v>
       </c>
       <c r="G41" t="s">
-        <v>99</v>
+        <v>437</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -3100,7 +2608,7 @@
         <v>11</v>
       </c>
       <c r="G42" t="s">
-        <v>104</v>
+        <v>438</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -3117,7 +2625,7 @@
         <v>105</v>
       </c>
       <c r="G43" t="s">
-        <v>104</v>
+        <v>438</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -3137,7 +2645,7 @@
         <v>50</v>
       </c>
       <c r="G44" t="s">
-        <v>107</v>
+        <v>439</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -3154,7 +2662,7 @@
         <v>108</v>
       </c>
       <c r="G45" t="s">
-        <v>107</v>
+        <v>439</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -3174,7 +2682,7 @@
         <v>50</v>
       </c>
       <c r="G46" t="s">
-        <v>112</v>
+        <v>440</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -3191,7 +2699,7 @@
         <v>113</v>
       </c>
       <c r="G47" t="s">
-        <v>112</v>
+        <v>440</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -3211,7 +2719,7 @@
         <v>115</v>
       </c>
       <c r="G48" t="s">
-        <v>116</v>
+        <v>441</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -3228,7 +2736,7 @@
         <v>117</v>
       </c>
       <c r="G49" t="s">
-        <v>116</v>
+        <v>441</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -3248,7 +2756,7 @@
         <v>11</v>
       </c>
       <c r="G50" t="s">
-        <v>121</v>
+        <v>442</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -3265,7 +2773,7 @@
         <v>122</v>
       </c>
       <c r="G51" t="s">
-        <v>121</v>
+        <v>442</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -3282,7 +2790,7 @@
         <v>124</v>
       </c>
       <c r="G52" t="s">
-        <v>123</v>
+        <v>443</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -3302,7 +2810,7 @@
         <v>62</v>
       </c>
       <c r="G53" t="s">
-        <v>123</v>
+        <v>443</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -3322,7 +2830,7 @@
         <v>11</v>
       </c>
       <c r="G54" t="s">
-        <v>626</v>
+        <v>444</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -3342,7 +2850,7 @@
         <v>50</v>
       </c>
       <c r="G55" t="s">
-        <v>627</v>
+        <v>445</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -3362,7 +2870,7 @@
         <v>62</v>
       </c>
       <c r="G56" t="s">
-        <v>622</v>
+        <v>429</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -3379,7 +2887,7 @@
         <v>128</v>
       </c>
       <c r="G57" t="s">
-        <v>626</v>
+        <v>444</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -3396,7 +2904,7 @@
         <v>130</v>
       </c>
       <c r="G58" t="s">
-        <v>627</v>
+        <v>445</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -3413,7 +2921,7 @@
         <v>132</v>
       </c>
       <c r="G59" t="s">
-        <v>622</v>
+        <v>429</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -3433,7 +2941,7 @@
         <v>11</v>
       </c>
       <c r="G60" t="s">
-        <v>135</v>
+        <v>446</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -3453,7 +2961,7 @@
         <v>50</v>
       </c>
       <c r="G61" t="s">
-        <v>136</v>
+        <v>447</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -3470,7 +2978,7 @@
         <v>137</v>
       </c>
       <c r="G62" t="s">
-        <v>136</v>
+        <v>447</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -3487,7 +2995,7 @@
         <v>138</v>
       </c>
       <c r="G63" t="s">
-        <v>135</v>
+        <v>446</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -3507,7 +3015,7 @@
         <v>11</v>
       </c>
       <c r="G64" t="s">
-        <v>141</v>
+        <v>448</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -3524,7 +3032,7 @@
         <v>142</v>
       </c>
       <c r="G65" t="s">
-        <v>141</v>
+        <v>448</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -3544,7 +3052,7 @@
         <v>11</v>
       </c>
       <c r="G66" t="s">
-        <v>145</v>
+        <v>449</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -3561,7 +3069,7 @@
         <v>146</v>
       </c>
       <c r="G67" t="s">
-        <v>145</v>
+        <v>449</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -3581,7 +3089,7 @@
         <v>11</v>
       </c>
       <c r="G68" t="s">
-        <v>149</v>
+        <v>450</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -3598,7 +3106,7 @@
         <v>150</v>
       </c>
       <c r="G69" t="s">
-        <v>149</v>
+        <v>450</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -3618,7 +3126,7 @@
         <v>11</v>
       </c>
       <c r="G70" t="s">
-        <v>153</v>
+        <v>451</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -3635,7 +3143,7 @@
         <v>154</v>
       </c>
       <c r="G71" t="s">
-        <v>153</v>
+        <v>451</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -3655,7 +3163,7 @@
         <v>11</v>
       </c>
       <c r="G72" t="s">
-        <v>157</v>
+        <v>452</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -3672,7 +3180,7 @@
         <v>158</v>
       </c>
       <c r="G73" t="s">
-        <v>157</v>
+        <v>452</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -3692,7 +3200,7 @@
         <v>11</v>
       </c>
       <c r="G74" t="s">
-        <v>161</v>
+        <v>453</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -3709,7 +3217,7 @@
         <v>162</v>
       </c>
       <c r="G75" t="s">
-        <v>161</v>
+        <v>453</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -3729,7 +3237,7 @@
         <v>11</v>
       </c>
       <c r="G76" t="s">
-        <v>165</v>
+        <v>454</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -3749,7 +3257,7 @@
         <v>50</v>
       </c>
       <c r="G77" t="s">
-        <v>166</v>
+        <v>455</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -3766,7 +3274,7 @@
         <v>167</v>
       </c>
       <c r="G78" t="s">
-        <v>165</v>
+        <v>454</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -3783,7 +3291,7 @@
         <v>168</v>
       </c>
       <c r="G79" t="s">
-        <v>166</v>
+        <v>455</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -3803,7 +3311,7 @@
         <v>11</v>
       </c>
       <c r="G80" t="s">
-        <v>172</v>
+        <v>456</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -3820,7 +3328,7 @@
         <v>173</v>
       </c>
       <c r="G81" t="s">
-        <v>172</v>
+        <v>456</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -3840,7 +3348,7 @@
         <v>62</v>
       </c>
       <c r="G82" t="s">
-        <v>174</v>
+        <v>457</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -3857,7 +3365,7 @@
         <v>175</v>
       </c>
       <c r="G83" t="s">
-        <v>174</v>
+        <v>457</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -4077,7 +3585,7 @@
         <v>11</v>
       </c>
       <c r="G95" t="s">
-        <v>621</v>
+        <v>458</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -4097,7 +3605,7 @@
         <v>62</v>
       </c>
       <c r="G96" t="s">
-        <v>622</v>
+        <v>459</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -4117,7 +3625,7 @@
         <v>11</v>
       </c>
       <c r="G97" t="s">
-        <v>620</v>
+        <v>416</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -4397,7 +3905,7 @@
         <v>11</v>
       </c>
       <c r="G111" t="s">
-        <v>626</v>
+        <v>460</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -4417,7 +3925,7 @@
         <v>50</v>
       </c>
       <c r="G112" t="s">
-        <v>627</v>
+        <v>461</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -4437,7 +3945,7 @@
         <v>62</v>
       </c>
       <c r="G113" t="s">
-        <v>622</v>
+        <v>459</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -4678,1278 +4186,6 @@
       </c>
       <c r="G125" t="s">
         <v>377</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>378</v>
-      </c>
-      <c r="B127" t="s">
-        <v>8</v>
-      </c>
-      <c r="C127" t="s">
-        <v>379</v>
-      </c>
-      <c r="D127" t="s">
-        <v>380</v>
-      </c>
-      <c r="E127" t="s">
-        <v>381</v>
-      </c>
-      <c r="G127" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>378</v>
-      </c>
-      <c r="B128" t="s">
-        <v>13</v>
-      </c>
-      <c r="C128" t="s">
-        <v>382</v>
-      </c>
-      <c r="F128" t="s">
-        <v>383</v>
-      </c>
-      <c r="G128" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>378</v>
-      </c>
-      <c r="B129" t="s">
-        <v>13</v>
-      </c>
-      <c r="C129" t="s">
-        <v>384</v>
-      </c>
-      <c r="F129" t="s">
-        <v>385</v>
-      </c>
-      <c r="G129" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>386</v>
-      </c>
-      <c r="B130" t="s">
-        <v>8</v>
-      </c>
-      <c r="C130" t="s">
-        <v>387</v>
-      </c>
-      <c r="D130" t="s">
-        <v>388</v>
-      </c>
-      <c r="E130" t="s">
-        <v>381</v>
-      </c>
-      <c r="G130" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>386</v>
-      </c>
-      <c r="B131" t="s">
-        <v>13</v>
-      </c>
-      <c r="C131" t="s">
-        <v>389</v>
-      </c>
-      <c r="F131" t="s">
-        <v>390</v>
-      </c>
-      <c r="G131" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>386</v>
-      </c>
-      <c r="B132" t="s">
-        <v>13</v>
-      </c>
-      <c r="C132" t="s">
-        <v>391</v>
-      </c>
-      <c r="F132" t="s">
-        <v>392</v>
-      </c>
-      <c r="G132" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>615</v>
-      </c>
-      <c r="B133" t="s">
-        <v>8</v>
-      </c>
-      <c r="C133" t="s">
-        <v>393</v>
-      </c>
-      <c r="D133" t="s">
-        <v>388</v>
-      </c>
-      <c r="E133" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>395</v>
-      </c>
-      <c r="B134" t="s">
-        <v>8</v>
-      </c>
-      <c r="C134" t="s">
-        <v>396</v>
-      </c>
-      <c r="D134" t="s">
-        <v>397</v>
-      </c>
-      <c r="E134" t="s">
-        <v>381</v>
-      </c>
-      <c r="G134" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>395</v>
-      </c>
-      <c r="B135" t="s">
-        <v>13</v>
-      </c>
-      <c r="C135" t="s">
-        <v>398</v>
-      </c>
-      <c r="F135" t="s">
-        <v>399</v>
-      </c>
-      <c r="G135" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>400</v>
-      </c>
-      <c r="B136" t="s">
-        <v>8</v>
-      </c>
-      <c r="C136" t="s">
-        <v>401</v>
-      </c>
-      <c r="D136" t="s">
-        <v>402</v>
-      </c>
-      <c r="E136" t="s">
-        <v>381</v>
-      </c>
-      <c r="G136" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>400</v>
-      </c>
-      <c r="B137" t="s">
-        <v>13</v>
-      </c>
-      <c r="C137" t="s">
-        <v>403</v>
-      </c>
-      <c r="F137" t="s">
-        <v>404</v>
-      </c>
-      <c r="G137" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>405</v>
-      </c>
-      <c r="B138" t="s">
-        <v>8</v>
-      </c>
-      <c r="C138" t="s">
-        <v>406</v>
-      </c>
-      <c r="D138" t="s">
-        <v>407</v>
-      </c>
-      <c r="E138" t="s">
-        <v>381</v>
-      </c>
-      <c r="G138" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>405</v>
-      </c>
-      <c r="B139" t="s">
-        <v>13</v>
-      </c>
-      <c r="C139" t="s">
-        <v>408</v>
-      </c>
-      <c r="F139" t="s">
-        <v>409</v>
-      </c>
-      <c r="G139" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>410</v>
-      </c>
-      <c r="B140" t="s">
-        <v>8</v>
-      </c>
-      <c r="C140" t="s">
-        <v>411</v>
-      </c>
-      <c r="D140" t="s">
-        <v>412</v>
-      </c>
-      <c r="E140" t="s">
-        <v>381</v>
-      </c>
-      <c r="G140" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>410</v>
-      </c>
-      <c r="B141" t="s">
-        <v>13</v>
-      </c>
-      <c r="C141" t="s">
-        <v>413</v>
-      </c>
-      <c r="F141" t="s">
-        <v>414</v>
-      </c>
-      <c r="G141" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>415</v>
-      </c>
-      <c r="B142" t="s">
-        <v>8</v>
-      </c>
-      <c r="C142" t="s">
-        <v>416</v>
-      </c>
-      <c r="D142" t="s">
-        <v>417</v>
-      </c>
-      <c r="E142" t="s">
-        <v>381</v>
-      </c>
-      <c r="G142" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>415</v>
-      </c>
-      <c r="B143" t="s">
-        <v>13</v>
-      </c>
-      <c r="C143" t="s">
-        <v>418</v>
-      </c>
-      <c r="F143" t="s">
-        <v>419</v>
-      </c>
-      <c r="G143" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>420</v>
-      </c>
-      <c r="B144" t="s">
-        <v>8</v>
-      </c>
-      <c r="C144" t="s">
-        <v>421</v>
-      </c>
-      <c r="D144" t="s">
-        <v>422</v>
-      </c>
-      <c r="E144" t="s">
-        <v>381</v>
-      </c>
-      <c r="G144" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>420</v>
-      </c>
-      <c r="B145" t="s">
-        <v>13</v>
-      </c>
-      <c r="C145" t="s">
-        <v>423</v>
-      </c>
-      <c r="F145" t="s">
-        <v>424</v>
-      </c>
-      <c r="G145" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>425</v>
-      </c>
-      <c r="B146" t="s">
-        <v>8</v>
-      </c>
-      <c r="C146" t="s">
-        <v>426</v>
-      </c>
-      <c r="D146" t="s">
-        <v>427</v>
-      </c>
-      <c r="E146" t="s">
-        <v>381</v>
-      </c>
-      <c r="G146" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>425</v>
-      </c>
-      <c r="B147" t="s">
-        <v>13</v>
-      </c>
-      <c r="C147" t="s">
-        <v>428</v>
-      </c>
-      <c r="F147" t="s">
-        <v>429</v>
-      </c>
-      <c r="G147" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>430</v>
-      </c>
-      <c r="B148" t="s">
-        <v>8</v>
-      </c>
-      <c r="C148" t="s">
-        <v>431</v>
-      </c>
-      <c r="D148" t="s">
-        <v>432</v>
-      </c>
-      <c r="E148" t="s">
-        <v>381</v>
-      </c>
-      <c r="G148" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>430</v>
-      </c>
-      <c r="B149" t="s">
-        <v>13</v>
-      </c>
-      <c r="C149" t="s">
-        <v>433</v>
-      </c>
-      <c r="F149" t="s">
-        <v>434</v>
-      </c>
-      <c r="G149" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>435</v>
-      </c>
-      <c r="B150" t="s">
-        <v>8</v>
-      </c>
-      <c r="C150" t="s">
-        <v>436</v>
-      </c>
-      <c r="D150" t="s">
-        <v>437</v>
-      </c>
-      <c r="E150" t="s">
-        <v>381</v>
-      </c>
-      <c r="G150" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>435</v>
-      </c>
-      <c r="B151" t="s">
-        <v>13</v>
-      </c>
-      <c r="C151" t="s">
-        <v>438</v>
-      </c>
-      <c r="F151" t="s">
-        <v>439</v>
-      </c>
-      <c r="G151" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>440</v>
-      </c>
-      <c r="B152" t="s">
-        <v>8</v>
-      </c>
-      <c r="C152" t="s">
-        <v>441</v>
-      </c>
-      <c r="D152" t="s">
-        <v>442</v>
-      </c>
-      <c r="E152" t="s">
-        <v>381</v>
-      </c>
-      <c r="G152" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>440</v>
-      </c>
-      <c r="B153" t="s">
-        <v>13</v>
-      </c>
-      <c r="C153" t="s">
-        <v>443</v>
-      </c>
-      <c r="F153" t="s">
-        <v>444</v>
-      </c>
-      <c r="G153" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>445</v>
-      </c>
-      <c r="B154" t="s">
-        <v>8</v>
-      </c>
-      <c r="C154" t="s">
-        <v>446</v>
-      </c>
-      <c r="D154" t="s">
-        <v>447</v>
-      </c>
-      <c r="E154" t="s">
-        <v>381</v>
-      </c>
-      <c r="G154" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>445</v>
-      </c>
-      <c r="B155" t="s">
-        <v>13</v>
-      </c>
-      <c r="C155" t="s">
-        <v>448</v>
-      </c>
-      <c r="F155" t="s">
-        <v>449</v>
-      </c>
-      <c r="G155" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>450</v>
-      </c>
-      <c r="B156" t="s">
-        <v>8</v>
-      </c>
-      <c r="C156" t="s">
-        <v>451</v>
-      </c>
-      <c r="D156" t="s">
-        <v>452</v>
-      </c>
-      <c r="E156" t="s">
-        <v>381</v>
-      </c>
-      <c r="G156" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>450</v>
-      </c>
-      <c r="B157" t="s">
-        <v>13</v>
-      </c>
-      <c r="C157" t="s">
-        <v>453</v>
-      </c>
-      <c r="F157" t="s">
-        <v>454</v>
-      </c>
-      <c r="G157" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>455</v>
-      </c>
-      <c r="B158" t="s">
-        <v>8</v>
-      </c>
-      <c r="C158" t="s">
-        <v>456</v>
-      </c>
-      <c r="D158" t="s">
-        <v>457</v>
-      </c>
-      <c r="E158" t="s">
-        <v>381</v>
-      </c>
-      <c r="G158" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>455</v>
-      </c>
-      <c r="B159" t="s">
-        <v>13</v>
-      </c>
-      <c r="C159" t="s">
-        <v>458</v>
-      </c>
-      <c r="F159" t="s">
-        <v>459</v>
-      </c>
-      <c r="G159" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>460</v>
-      </c>
-      <c r="B160" t="s">
-        <v>8</v>
-      </c>
-      <c r="C160" t="s">
-        <v>461</v>
-      </c>
-      <c r="D160" t="s">
-        <v>462</v>
-      </c>
-      <c r="E160" t="s">
-        <v>381</v>
-      </c>
-      <c r="G160" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>460</v>
-      </c>
-      <c r="B161" t="s">
-        <v>13</v>
-      </c>
-      <c r="C161" t="s">
-        <v>463</v>
-      </c>
-      <c r="F161" t="s">
-        <v>464</v>
-      </c>
-      <c r="G161" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>465</v>
-      </c>
-      <c r="B162" t="s">
-        <v>8</v>
-      </c>
-      <c r="C162" t="s">
-        <v>466</v>
-      </c>
-      <c r="D162" t="s">
-        <v>467</v>
-      </c>
-      <c r="E162" t="s">
-        <v>381</v>
-      </c>
-      <c r="G162" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>465</v>
-      </c>
-      <c r="B163" t="s">
-        <v>13</v>
-      </c>
-      <c r="C163" t="s">
-        <v>468</v>
-      </c>
-      <c r="F163" t="s">
-        <v>469</v>
-      </c>
-      <c r="G163" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>470</v>
-      </c>
-      <c r="B164" t="s">
-        <v>8</v>
-      </c>
-      <c r="C164" t="s">
-        <v>471</v>
-      </c>
-      <c r="D164" t="s">
-        <v>472</v>
-      </c>
-      <c r="E164" t="s">
-        <v>381</v>
-      </c>
-      <c r="G164" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>470</v>
-      </c>
-      <c r="B165" t="s">
-        <v>13</v>
-      </c>
-      <c r="C165" t="s">
-        <v>473</v>
-      </c>
-      <c r="F165" t="s">
-        <v>474</v>
-      </c>
-      <c r="G165" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>475</v>
-      </c>
-      <c r="B166" t="s">
-        <v>8</v>
-      </c>
-      <c r="C166" t="s">
-        <v>476</v>
-      </c>
-      <c r="D166" t="s">
-        <v>477</v>
-      </c>
-      <c r="E166" t="s">
-        <v>381</v>
-      </c>
-      <c r="G166" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>475</v>
-      </c>
-      <c r="B167" t="s">
-        <v>13</v>
-      </c>
-      <c r="C167" t="s">
-        <v>478</v>
-      </c>
-      <c r="F167" t="s">
-        <v>479</v>
-      </c>
-      <c r="G167" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>480</v>
-      </c>
-      <c r="B168" t="s">
-        <v>8</v>
-      </c>
-      <c r="C168" t="s">
-        <v>481</v>
-      </c>
-      <c r="D168" t="s">
-        <v>482</v>
-      </c>
-      <c r="E168" t="s">
-        <v>381</v>
-      </c>
-      <c r="G168" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
-        <v>480</v>
-      </c>
-      <c r="B169" t="s">
-        <v>13</v>
-      </c>
-      <c r="C169" t="s">
-        <v>483</v>
-      </c>
-      <c r="F169" t="s">
-        <v>484</v>
-      </c>
-      <c r="G169" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>485</v>
-      </c>
-      <c r="B170" t="s">
-        <v>8</v>
-      </c>
-      <c r="C170" t="s">
-        <v>486</v>
-      </c>
-      <c r="D170" t="s">
-        <v>487</v>
-      </c>
-      <c r="E170" t="s">
-        <v>381</v>
-      </c>
-      <c r="G170" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>485</v>
-      </c>
-      <c r="B171" t="s">
-        <v>13</v>
-      </c>
-      <c r="C171" t="s">
-        <v>488</v>
-      </c>
-      <c r="F171" t="s">
-        <v>489</v>
-      </c>
-      <c r="G171" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>490</v>
-      </c>
-      <c r="B172" t="s">
-        <v>8</v>
-      </c>
-      <c r="C172" t="s">
-        <v>491</v>
-      </c>
-      <c r="D172" t="s">
-        <v>492</v>
-      </c>
-      <c r="E172" t="s">
-        <v>381</v>
-      </c>
-      <c r="G172" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>490</v>
-      </c>
-      <c r="B173" t="s">
-        <v>13</v>
-      </c>
-      <c r="C173" t="s">
-        <v>493</v>
-      </c>
-      <c r="F173" t="s">
-        <v>494</v>
-      </c>
-      <c r="G173" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
-        <v>495</v>
-      </c>
-      <c r="B174" t="s">
-        <v>8</v>
-      </c>
-      <c r="C174" t="s">
-        <v>496</v>
-      </c>
-      <c r="D174" t="s">
-        <v>497</v>
-      </c>
-      <c r="E174" t="s">
-        <v>381</v>
-      </c>
-      <c r="G174" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
-        <v>495</v>
-      </c>
-      <c r="B175" t="s">
-        <v>13</v>
-      </c>
-      <c r="C175" t="s">
-        <v>498</v>
-      </c>
-      <c r="F175" t="s">
-        <v>499</v>
-      </c>
-      <c r="G175" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
-        <v>500</v>
-      </c>
-      <c r="B176" t="s">
-        <v>8</v>
-      </c>
-      <c r="C176" t="s">
-        <v>501</v>
-      </c>
-      <c r="D176" t="s">
-        <v>502</v>
-      </c>
-      <c r="E176" t="s">
-        <v>381</v>
-      </c>
-      <c r="G176" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>500</v>
-      </c>
-      <c r="B177" t="s">
-        <v>13</v>
-      </c>
-      <c r="C177" t="s">
-        <v>503</v>
-      </c>
-      <c r="F177" t="s">
-        <v>504</v>
-      </c>
-      <c r="G177" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>505</v>
-      </c>
-      <c r="B178" t="s">
-        <v>8</v>
-      </c>
-      <c r="C178" t="s">
-        <v>506</v>
-      </c>
-      <c r="D178" t="s">
-        <v>507</v>
-      </c>
-      <c r="E178" t="s">
-        <v>381</v>
-      </c>
-      <c r="G178" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>505</v>
-      </c>
-      <c r="B179" t="s">
-        <v>13</v>
-      </c>
-      <c r="C179" t="s">
-        <v>508</v>
-      </c>
-      <c r="F179" t="s">
-        <v>509</v>
-      </c>
-      <c r="G179" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>510</v>
-      </c>
-      <c r="B180" t="s">
-        <v>8</v>
-      </c>
-      <c r="C180" t="s">
-        <v>511</v>
-      </c>
-      <c r="D180" t="s">
-        <v>512</v>
-      </c>
-      <c r="E180" t="s">
-        <v>381</v>
-      </c>
-      <c r="G180" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>510</v>
-      </c>
-      <c r="B181" t="s">
-        <v>13</v>
-      </c>
-      <c r="C181" t="s">
-        <v>513</v>
-      </c>
-      <c r="F181" t="s">
-        <v>514</v>
-      </c>
-      <c r="G181" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>515</v>
-      </c>
-      <c r="B182" t="s">
-        <v>8</v>
-      </c>
-      <c r="C182" t="s">
-        <v>481</v>
-      </c>
-      <c r="D182" t="s">
-        <v>516</v>
-      </c>
-      <c r="E182" t="s">
-        <v>381</v>
-      </c>
-      <c r="G182" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>515</v>
-      </c>
-      <c r="B183" t="s">
-        <v>13</v>
-      </c>
-      <c r="C183" t="s">
-        <v>517</v>
-      </c>
-      <c r="F183" t="s">
-        <v>518</v>
-      </c>
-      <c r="G183" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
-        <v>519</v>
-      </c>
-      <c r="B184" t="s">
-        <v>8</v>
-      </c>
-      <c r="C184" t="s">
-        <v>520</v>
-      </c>
-      <c r="D184" t="s">
-        <v>521</v>
-      </c>
-      <c r="E184" t="s">
-        <v>381</v>
-      </c>
-      <c r="G184" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>519</v>
-      </c>
-      <c r="B185" t="s">
-        <v>13</v>
-      </c>
-      <c r="C185" t="s">
-        <v>522</v>
-      </c>
-      <c r="F185" t="s">
-        <v>523</v>
-      </c>
-      <c r="G185" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
-        <v>524</v>
-      </c>
-      <c r="B186" t="s">
-        <v>8</v>
-      </c>
-      <c r="C186" t="s">
-        <v>525</v>
-      </c>
-      <c r="D186" t="s">
-        <v>526</v>
-      </c>
-      <c r="E186" t="s">
-        <v>381</v>
-      </c>
-      <c r="G186" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
-        <v>524</v>
-      </c>
-      <c r="B187" t="s">
-        <v>13</v>
-      </c>
-      <c r="C187" t="s">
-        <v>527</v>
-      </c>
-      <c r="F187" t="s">
-        <v>528</v>
-      </c>
-      <c r="G187" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
-        <v>529</v>
-      </c>
-      <c r="B188" t="s">
-        <v>8</v>
-      </c>
-      <c r="C188" t="s">
-        <v>530</v>
-      </c>
-      <c r="D188" t="s">
-        <v>531</v>
-      </c>
-      <c r="E188" t="s">
-        <v>381</v>
-      </c>
-      <c r="G188" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>529</v>
-      </c>
-      <c r="B189" t="s">
-        <v>13</v>
-      </c>
-      <c r="C189" t="s">
-        <v>532</v>
-      </c>
-      <c r="F189" t="s">
-        <v>533</v>
-      </c>
-      <c r="G189" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
-        <v>534</v>
-      </c>
-      <c r="B190" t="s">
-        <v>8</v>
-      </c>
-      <c r="C190" t="s">
-        <v>535</v>
-      </c>
-      <c r="D190" t="s">
-        <v>536</v>
-      </c>
-      <c r="E190" t="s">
-        <v>381</v>
-      </c>
-      <c r="G190" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
-        <v>534</v>
-      </c>
-      <c r="B191" t="s">
-        <v>13</v>
-      </c>
-      <c r="C191" t="s">
-        <v>537</v>
-      </c>
-      <c r="F191" t="s">
-        <v>538</v>
-      </c>
-      <c r="G191" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
-        <v>539</v>
-      </c>
-      <c r="B192" t="s">
-        <v>8</v>
-      </c>
-      <c r="C192" t="s">
-        <v>540</v>
-      </c>
-      <c r="D192" t="s">
-        <v>541</v>
-      </c>
-      <c r="E192" t="s">
-        <v>381</v>
-      </c>
-      <c r="G192" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
-        <v>539</v>
-      </c>
-      <c r="B193" t="s">
-        <v>13</v>
-      </c>
-      <c r="C193" t="s">
-        <v>542</v>
-      </c>
-      <c r="F193" t="s">
-        <v>543</v>
-      </c>
-      <c r="G193" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
-        <v>544</v>
-      </c>
-      <c r="B194" t="s">
-        <v>8</v>
-      </c>
-      <c r="C194" t="s">
-        <v>545</v>
-      </c>
-      <c r="D194" t="s">
-        <v>546</v>
-      </c>
-      <c r="E194" t="s">
-        <v>381</v>
-      </c>
-      <c r="G194" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
-        <v>544</v>
-      </c>
-      <c r="B195" t="s">
-        <v>13</v>
-      </c>
-      <c r="C195" t="s">
-        <v>547</v>
-      </c>
-      <c r="F195" t="s">
-        <v>548</v>
-      </c>
-      <c r="G195" t="s">
-        <v>547</v>
       </c>
     </row>
   </sheetData>
@@ -5962,8 +4198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6005,10 +4241,10 @@
         <v>182</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>624</v>
+        <v>462</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>625</v>
+        <v>463</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>183</v>
@@ -6129,7 +4365,7 @@
         <v>188</v>
       </c>
       <c r="H6" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -6152,7 +4388,7 @@
         <v>188</v>
       </c>
       <c r="H7" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -6175,7 +4411,7 @@
         <v>188</v>
       </c>
       <c r="H8" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -6198,7 +4434,7 @@
         <v>188</v>
       </c>
       <c r="H9" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -6221,7 +4457,7 @@
         <v>188</v>
       </c>
       <c r="H10" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -6267,7 +4503,7 @@
         <v>188</v>
       </c>
       <c r="H12" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -6313,7 +4549,7 @@
         <v>188</v>
       </c>
       <c r="H14" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -6336,7 +4572,7 @@
         <v>188</v>
       </c>
       <c r="H15" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -6359,7 +4595,7 @@
         <v>188</v>
       </c>
       <c r="H16" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -6382,7 +4618,7 @@
         <v>188</v>
       </c>
       <c r="H17" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -6405,7 +4641,7 @@
         <v>188</v>
       </c>
       <c r="H18" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -6441,9 +4677,6 @@
       <c r="C20" t="s">
         <v>185</v>
       </c>
-      <c r="D20" t="s">
-        <v>120</v>
-      </c>
       <c r="E20" t="s">
         <v>186</v>
       </c>
@@ -6457,7 +4690,7 @@
         <v>190</v>
       </c>
       <c r="I20" t="s">
-        <v>623</v>
+        <v>417</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -6503,7 +4736,7 @@
         <v>188</v>
       </c>
       <c r="H22" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -6526,7 +4759,7 @@
         <v>188</v>
       </c>
       <c r="H23" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -6549,7 +4782,7 @@
         <v>188</v>
       </c>
       <c r="H24" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -6572,7 +4805,7 @@
         <v>188</v>
       </c>
       <c r="H25" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -6595,7 +4828,7 @@
         <v>188</v>
       </c>
       <c r="H26" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -6618,7 +4851,7 @@
         <v>188</v>
       </c>
       <c r="H27" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -6641,7 +4874,7 @@
         <v>188</v>
       </c>
       <c r="H28" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -6664,7 +4897,7 @@
         <v>188</v>
       </c>
       <c r="H29" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -6715,22 +4948,22 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B33" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="C33" t="s">
         <v>185</v>
       </c>
       <c r="D33" t="s">
-        <v>617</v>
+        <v>413</v>
       </c>
       <c r="E33" t="s">
         <v>186</v>
       </c>
       <c r="F33" t="s">
-        <v>549</v>
+        <v>411</v>
       </c>
       <c r="G33" t="s">
         <v>188</v>
@@ -6741,22 +4974,22 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>615</v>
+        <v>412</v>
       </c>
       <c r="B34" t="s">
-        <v>615</v>
+        <v>412</v>
       </c>
       <c r="C34" t="s">
         <v>185</v>
       </c>
       <c r="D34" t="s">
-        <v>618</v>
+        <v>414</v>
       </c>
       <c r="E34" t="s">
         <v>186</v>
       </c>
       <c r="F34" t="s">
-        <v>619</v>
+        <v>415</v>
       </c>
       <c r="G34" t="s">
         <v>188</v>
@@ -6767,10 +5000,10 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
       <c r="B35" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
       <c r="C35" t="s">
         <v>185</v>
@@ -6790,10 +5023,10 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>400</v>
+        <v>381</v>
       </c>
       <c r="B36" t="s">
-        <v>400</v>
+        <v>381</v>
       </c>
       <c r="C36" t="s">
         <v>185</v>
@@ -6802,7 +5035,7 @@
         <v>186</v>
       </c>
       <c r="F36" t="s">
-        <v>549</v>
+        <v>411</v>
       </c>
       <c r="G36" t="s">
         <v>188</v>
@@ -6813,10 +5046,10 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>405</v>
+        <v>382</v>
       </c>
       <c r="B37" t="s">
-        <v>405</v>
+        <v>382</v>
       </c>
       <c r="C37" t="s">
         <v>185</v>
@@ -6836,10 +5069,10 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>410</v>
+        <v>383</v>
       </c>
       <c r="B38" t="s">
-        <v>410</v>
+        <v>383</v>
       </c>
       <c r="C38" t="s">
         <v>185</v>
@@ -6859,10 +5092,10 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>415</v>
+        <v>384</v>
       </c>
       <c r="B39" t="s">
-        <v>415</v>
+        <v>384</v>
       </c>
       <c r="C39" t="s">
         <v>185</v>
@@ -6882,10 +5115,10 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>420</v>
+        <v>385</v>
       </c>
       <c r="B40" t="s">
-        <v>420</v>
+        <v>385</v>
       </c>
       <c r="C40" t="s">
         <v>185</v>
@@ -6905,10 +5138,10 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>425</v>
+        <v>386</v>
       </c>
       <c r="B41" t="s">
-        <v>425</v>
+        <v>386</v>
       </c>
       <c r="C41" t="s">
         <v>185</v>
@@ -6928,10 +5161,10 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>430</v>
+        <v>387</v>
       </c>
       <c r="B42" t="s">
-        <v>430</v>
+        <v>387</v>
       </c>
       <c r="C42" t="s">
         <v>185</v>
@@ -6951,10 +5184,10 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>435</v>
+        <v>388</v>
       </c>
       <c r="B43" t="s">
-        <v>435</v>
+        <v>388</v>
       </c>
       <c r="C43" t="s">
         <v>185</v>
@@ -6974,10 +5207,10 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>440</v>
+        <v>389</v>
       </c>
       <c r="B44" t="s">
-        <v>440</v>
+        <v>389</v>
       </c>
       <c r="C44" t="s">
         <v>185</v>
@@ -6997,10 +5230,10 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>445</v>
+        <v>390</v>
       </c>
       <c r="B45" t="s">
-        <v>445</v>
+        <v>390</v>
       </c>
       <c r="C45" t="s">
         <v>185</v>
@@ -7020,10 +5253,10 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>450</v>
+        <v>391</v>
       </c>
       <c r="B46" t="s">
-        <v>450</v>
+        <v>391</v>
       </c>
       <c r="C46" t="s">
         <v>185</v>
@@ -7043,10 +5276,10 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>455</v>
+        <v>392</v>
       </c>
       <c r="B47" t="s">
-        <v>455</v>
+        <v>392</v>
       </c>
       <c r="C47" t="s">
         <v>185</v>
@@ -7066,10 +5299,10 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>460</v>
+        <v>393</v>
       </c>
       <c r="B48" t="s">
-        <v>460</v>
+        <v>393</v>
       </c>
       <c r="C48" t="s">
         <v>185</v>
@@ -7089,10 +5322,10 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>465</v>
+        <v>394</v>
       </c>
       <c r="B49" t="s">
-        <v>465</v>
+        <v>394</v>
       </c>
       <c r="C49" t="s">
         <v>185</v>
@@ -7112,10 +5345,10 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>470</v>
+        <v>395</v>
       </c>
       <c r="B50" t="s">
-        <v>470</v>
+        <v>395</v>
       </c>
       <c r="C50" t="s">
         <v>185</v>
@@ -7135,10 +5368,10 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>475</v>
+        <v>396</v>
       </c>
       <c r="B51" t="s">
-        <v>475</v>
+        <v>396</v>
       </c>
       <c r="C51" t="s">
         <v>185</v>
@@ -7147,7 +5380,7 @@
         <v>186</v>
       </c>
       <c r="F51" t="s">
-        <v>549</v>
+        <v>411</v>
       </c>
       <c r="G51" t="s">
         <v>188</v>
@@ -7158,10 +5391,10 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>480</v>
+        <v>397</v>
       </c>
       <c r="B52" t="s">
-        <v>480</v>
+        <v>397</v>
       </c>
       <c r="C52" t="s">
         <v>185</v>
@@ -7181,10 +5414,10 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>485</v>
+        <v>398</v>
       </c>
       <c r="B53" t="s">
-        <v>485</v>
+        <v>398</v>
       </c>
       <c r="C53" t="s">
         <v>185</v>
@@ -7204,10 +5437,10 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>490</v>
+        <v>399</v>
       </c>
       <c r="B54" t="s">
-        <v>490</v>
+        <v>399</v>
       </c>
       <c r="C54" t="s">
         <v>185</v>
@@ -7227,10 +5460,10 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>495</v>
+        <v>400</v>
       </c>
       <c r="B55" t="s">
-        <v>495</v>
+        <v>400</v>
       </c>
       <c r="C55" t="s">
         <v>185</v>
@@ -7250,10 +5483,10 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>500</v>
+        <v>401</v>
       </c>
       <c r="B56" t="s">
-        <v>500</v>
+        <v>401</v>
       </c>
       <c r="C56" t="s">
         <v>185</v>
@@ -7273,10 +5506,10 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>505</v>
+        <v>402</v>
       </c>
       <c r="B57" t="s">
-        <v>505</v>
+        <v>402</v>
       </c>
       <c r="C57" t="s">
         <v>185</v>
@@ -7296,10 +5529,10 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>510</v>
+        <v>403</v>
       </c>
       <c r="B58" t="s">
-        <v>510</v>
+        <v>403</v>
       </c>
       <c r="C58" t="s">
         <v>185</v>
@@ -7319,10 +5552,10 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>515</v>
+        <v>404</v>
       </c>
       <c r="B59" t="s">
-        <v>515</v>
+        <v>404</v>
       </c>
       <c r="C59" t="s">
         <v>185</v>
@@ -7342,10 +5575,10 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>519</v>
+        <v>405</v>
       </c>
       <c r="B60" t="s">
-        <v>519</v>
+        <v>405</v>
       </c>
       <c r="C60" t="s">
         <v>185</v>
@@ -7365,10 +5598,10 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>524</v>
+        <v>406</v>
       </c>
       <c r="B61" t="s">
-        <v>524</v>
+        <v>406</v>
       </c>
       <c r="C61" t="s">
         <v>185</v>
@@ -7388,10 +5621,10 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>529</v>
+        <v>407</v>
       </c>
       <c r="B62" t="s">
-        <v>529</v>
+        <v>407</v>
       </c>
       <c r="C62" t="s">
         <v>185</v>
@@ -7411,10 +5644,10 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>534</v>
+        <v>408</v>
       </c>
       <c r="B63" t="s">
-        <v>534</v>
+        <v>408</v>
       </c>
       <c r="C63" t="s">
         <v>185</v>
@@ -7434,10 +5667,10 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>539</v>
+        <v>409</v>
       </c>
       <c r="B64" t="s">
-        <v>539</v>
+        <v>409</v>
       </c>
       <c r="C64" t="s">
         <v>185</v>
@@ -7457,10 +5690,10 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>544</v>
+        <v>410</v>
       </c>
       <c r="B65" t="s">
-        <v>544</v>
+        <v>410</v>
       </c>
       <c r="C65" t="s">
         <v>185</v>
@@ -7485,10 +5718,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7828,369 +6061,6 @@
         <v>223</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>380</v>
-      </c>
-      <c r="B32" t="s">
-        <v>550</v>
-      </c>
-      <c r="C32" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>388</v>
-      </c>
-      <c r="B33" t="s">
-        <v>616</v>
-      </c>
-      <c r="C33" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>397</v>
-      </c>
-      <c r="B34" t="s">
-        <v>553</v>
-      </c>
-      <c r="C34" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>402</v>
-      </c>
-      <c r="B35" t="s">
-        <v>555</v>
-      </c>
-      <c r="C35" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>407</v>
-      </c>
-      <c r="B36" t="s">
-        <v>557</v>
-      </c>
-      <c r="C36" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>412</v>
-      </c>
-      <c r="B37" t="s">
-        <v>559</v>
-      </c>
-      <c r="C37" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>417</v>
-      </c>
-      <c r="B38" t="s">
-        <v>561</v>
-      </c>
-      <c r="C38" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>422</v>
-      </c>
-      <c r="B39" t="s">
-        <v>563</v>
-      </c>
-      <c r="C39" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>427</v>
-      </c>
-      <c r="B40" t="s">
-        <v>565</v>
-      </c>
-      <c r="C40" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>432</v>
-      </c>
-      <c r="B41" t="s">
-        <v>567</v>
-      </c>
-      <c r="C41" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>437</v>
-      </c>
-      <c r="B42" t="s">
-        <v>569</v>
-      </c>
-      <c r="C42" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>442</v>
-      </c>
-      <c r="B43" t="s">
-        <v>571</v>
-      </c>
-      <c r="C43" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>447</v>
-      </c>
-      <c r="B44" t="s">
-        <v>573</v>
-      </c>
-      <c r="C44" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>452</v>
-      </c>
-      <c r="B45" t="s">
-        <v>575</v>
-      </c>
-      <c r="C45" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>457</v>
-      </c>
-      <c r="B46" t="s">
-        <v>577</v>
-      </c>
-      <c r="C46" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>462</v>
-      </c>
-      <c r="B47" t="s">
-        <v>579</v>
-      </c>
-      <c r="C47" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>467</v>
-      </c>
-      <c r="B48" t="s">
-        <v>581</v>
-      </c>
-      <c r="C48" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>472</v>
-      </c>
-      <c r="B49" t="s">
-        <v>583</v>
-      </c>
-      <c r="C49" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>477</v>
-      </c>
-      <c r="B50" t="s">
-        <v>585</v>
-      </c>
-      <c r="C50" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>482</v>
-      </c>
-      <c r="B51" t="s">
-        <v>587</v>
-      </c>
-      <c r="C51" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>487</v>
-      </c>
-      <c r="B52" t="s">
-        <v>589</v>
-      </c>
-      <c r="C52" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>492</v>
-      </c>
-      <c r="B53" t="s">
-        <v>591</v>
-      </c>
-      <c r="C53" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>497</v>
-      </c>
-      <c r="B54" t="s">
-        <v>593</v>
-      </c>
-      <c r="C54" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>502</v>
-      </c>
-      <c r="B55" t="s">
-        <v>595</v>
-      </c>
-      <c r="C55" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>507</v>
-      </c>
-      <c r="B56" t="s">
-        <v>597</v>
-      </c>
-      <c r="C56" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>512</v>
-      </c>
-      <c r="B57" t="s">
-        <v>599</v>
-      </c>
-      <c r="C57" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>516</v>
-      </c>
-      <c r="B58" t="s">
-        <v>601</v>
-      </c>
-      <c r="C58" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>521</v>
-      </c>
-      <c r="B59" t="s">
-        <v>603</v>
-      </c>
-      <c r="C59" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>526</v>
-      </c>
-      <c r="B60" t="s">
-        <v>605</v>
-      </c>
-      <c r="C60" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>531</v>
-      </c>
-      <c r="B61" t="s">
-        <v>607</v>
-      </c>
-      <c r="C61" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>536</v>
-      </c>
-      <c r="B62" t="s">
-        <v>609</v>
-      </c>
-      <c r="C62" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>541</v>
-      </c>
-      <c r="B63" t="s">
-        <v>611</v>
-      </c>
-      <c r="C63" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>546</v>
-      </c>
-      <c r="B64" t="s">
-        <v>613</v>
-      </c>
-      <c r="C64" t="s">
-        <v>614</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -8199,10 +6069,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{672247AF-8ED4-4526-A66A-F7939ABE75ED}">
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8220,502 +6090,6 @@
       </c>
       <c r="C1" t="s">
         <v>267</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>77</v>
-      </c>
-      <c r="B13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>89</v>
-      </c>
-      <c r="B15" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>93</v>
-      </c>
-      <c r="B16" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>98</v>
-      </c>
-      <c r="B17" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>103</v>
-      </c>
-      <c r="B18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>111</v>
-      </c>
-      <c r="B19" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>120</v>
-      </c>
-      <c r="B20" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B21" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>134</v>
-      </c>
-      <c r="B22" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>140</v>
-      </c>
-      <c r="B23" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>144</v>
-      </c>
-      <c r="B24" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>148</v>
-      </c>
-      <c r="B25" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>152</v>
-      </c>
-      <c r="B26" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>156</v>
-      </c>
-      <c r="B27" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>160</v>
-      </c>
-      <c r="B28" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>164</v>
-      </c>
-      <c r="B29" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>171</v>
-      </c>
-      <c r="B30" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>380</v>
-      </c>
-      <c r="B32" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>388</v>
-      </c>
-      <c r="B33" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>397</v>
-      </c>
-      <c r="B34" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>402</v>
-      </c>
-      <c r="B35" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>407</v>
-      </c>
-      <c r="B36" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>412</v>
-      </c>
-      <c r="B37" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>417</v>
-      </c>
-      <c r="B38" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>422</v>
-      </c>
-      <c r="B39" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>427</v>
-      </c>
-      <c r="B40" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>432</v>
-      </c>
-      <c r="B41" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>437</v>
-      </c>
-      <c r="B42" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>442</v>
-      </c>
-      <c r="B43" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>447</v>
-      </c>
-      <c r="B44" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>452</v>
-      </c>
-      <c r="B45" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>457</v>
-      </c>
-      <c r="B46" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>462</v>
-      </c>
-      <c r="B47" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>467</v>
-      </c>
-      <c r="B48" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>472</v>
-      </c>
-      <c r="B49" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>477</v>
-      </c>
-      <c r="B50" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>482</v>
-      </c>
-      <c r="B51" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>487</v>
-      </c>
-      <c r="B52" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>492</v>
-      </c>
-      <c r="B53" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>497</v>
-      </c>
-      <c r="B54" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>502</v>
-      </c>
-      <c r="B55" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>507</v>
-      </c>
-      <c r="B56" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>512</v>
-      </c>
-      <c r="B57" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>516</v>
-      </c>
-      <c r="B58" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>521</v>
-      </c>
-      <c r="B59" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>526</v>
-      </c>
-      <c r="B60" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>531</v>
-      </c>
-      <c r="B61" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>536</v>
-      </c>
-      <c r="B62" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>541</v>
-      </c>
-      <c r="B63" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>546</v>
-      </c>
-      <c r="B64" t="s">
-        <v>546</v>
       </c>
     </row>
   </sheetData>
@@ -8733,6 +6107,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="425f6c96-429f-484f-969b-f607df711986">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="dffc3f26-5269-4005-8a8e-580fd4bf242e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100F7723F256106FF48A4FBBA5559F2847E" ma:contentTypeVersion="9" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="6dfbbd5d754489e869e2fe9e3db2ec32">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="425f6c96-429f-484f-969b-f607df711986" xmlns:ns3="dffc3f26-5269-4005-8a8e-580fd4bf242e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9bf0db8cee733190e30b0331135d530d" ns2:_="" ns3:_="">
     <xsd:import namespace="425f6c96-429f-484f-969b-f607df711986"/>
@@ -8915,17 +6300,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="425f6c96-429f-484f-969b-f607df711986">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="dffc3f26-5269-4005-8a8e-580fd4bf242e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CADC4558-0949-4370-ACA0-2191199EE721}">
   <ds:schemaRefs>
@@ -8935,6 +6309,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2AA2CE2D-DA25-4B4D-AC24-7B51966E82CB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="425f6c96-429f-484f-969b-f607df711986"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="dffc3f26-5269-4005-8a8e-580fd4bf242e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F068740D-A5A4-4E30-9F7B-8E99CA6C009C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8951,21 +6342,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2AA2CE2D-DA25-4B4D-AC24-7B51966E82CB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="425f6c96-429f-484f-969b-f607df711986"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="dffc3f26-5269-4005-8a8e-580fd4bf242e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>